<commit_message>
Added load function, cheatsheet, player-colored tabs, major and minor bug fixes
</commit_message>
<xml_diff>
--- a/Documenten/TO DO.xlsx
+++ b/Documenten/TO DO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Dropbox\RealLifeRiskR\shiny\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Documents\GitHub\RealLifeRisk\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
   <si>
     <t>TO DO</t>
   </si>
@@ -153,6 +153,39 @@
   </si>
   <si>
     <t>Nu zit de belangrijkste scripts in /Shiny en /Shiny/www. Het zou makkelijker zijn als de settings.xlsx een logischere naam heeft</t>
+  </si>
+  <si>
+    <t>Settings scherm afmaken</t>
+  </si>
+  <si>
+    <t>Load game inbouwen</t>
+  </si>
+  <si>
+    <t>Zorgen dat je een saved game kan inladen, zodat je verder kunt spelen na een crash en/of makkelijk terug kan naar een oude spelsituatie</t>
+  </si>
+  <si>
+    <t>Is nu puur visueel. Dit kan beter.</t>
+  </si>
+  <si>
+    <t>End-game credits inbouwen</t>
+  </si>
+  <si>
+    <t>Dit moet gewoon ;)</t>
+  </si>
+  <si>
+    <t>Notities</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>18-02-2020</t>
   </si>
 </sst>
 </file>
@@ -168,7 +201,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -184,6 +217,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -209,13 +254,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,29 +544,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="46.28515625" customWidth="1"/>
     <col min="3" max="3" width="181.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C2" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -528,8 +581,17 @@
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -539,8 +601,14 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="6">
+        <v>44959</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -550,8 +618,14 @@
       <c r="C5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="6">
+        <v>44959</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -562,7 +636,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -573,7 +647,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -584,7 +658,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -595,7 +669,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -606,7 +680,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -617,7 +691,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -628,7 +702,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -639,7 +713,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -649,8 +723,14 @@
       <c r="C14" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -660,8 +740,14 @@
       <c r="C15" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="6">
+        <v>44959</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
@@ -672,7 +758,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
@@ -682,8 +768,14 @@
       <c r="C17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="6">
+        <v>44959</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
@@ -694,7 +786,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
@@ -705,7 +797,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
@@ -715,8 +807,14 @@
       <c r="C20" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" s="6">
+        <v>44959</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
@@ -727,7 +825,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
@@ -736,6 +834,63 @@
       </c>
       <c r="C22" t="s">
         <v>42</v>
+      </c>
+      <c r="F22" t="s">
+        <v>52</v>
+      </c>
+      <c r="G22" s="6">
+        <v>44959</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" s="6">
+        <v>44959</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" t="s">
+        <v>52</v>
+      </c>
+      <c r="G24" s="6">
+        <v>44959</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25" s="6">
+        <v>44959</v>
       </c>
     </row>
   </sheetData>

</xml_diff>